<commit_message>
Updated header: Removed triangle, kept logo
</commit_message>
<xml_diff>
--- a/product list.xlsx
+++ b/product list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahtamiandashti/product-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C5C012-AFEB-0243-9A0D-3C2EB54E086B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B009FE1-C8A6-624F-88AE-72F727FBB270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
     <definedName name="Dialyzer_Name">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -1209,7 +1210,7 @@
   <dimension ref="A1:D176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3263,6 +3264,7 @@
       <c r="D176" s="9"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{17F5C3D3-4489-534F-B22E-FFEEBED3B745}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated full code with review page and product detail dropdown
</commit_message>
<xml_diff>
--- a/product list.xlsx
+++ b/product list.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahtamiandashti/product-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B009FE1-C8A6-624F-88AE-72F727FBB270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFF45E7-2F7D-964B-8BEF-DC6CCAECCDEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="21680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$124</definedName>
     <definedName name="Dialyzer_Name">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -53,87 +53,45 @@
     <t>NephroPS10R</t>
   </si>
   <si>
-    <t>NephroPS10R- Polysulfone Hemodialyzer 1.0 m2, Low Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS13R</t>
   </si>
   <si>
-    <t>NephroPS13R- Polysulfone Hemodialyzer 1.3 m2, Low Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS14R</t>
   </si>
   <si>
-    <t>NephroPS14R- Polysulfone Hemodialyzer 1.4 m2, Low Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS16R</t>
   </si>
   <si>
-    <t>NephroPS16R- Polysulfone Hemodialyzer 1.6 m2, Low Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS18R</t>
   </si>
   <si>
-    <t>NephroPS18R- Polysulfone Hemodialyzer 1.8 m2, Low Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS20R</t>
   </si>
   <si>
-    <t>NephroPS20R- Polysulfone Hemodialyzer 2.0 m2, Low Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS22R</t>
   </si>
   <si>
-    <t>NephroPS22R- Polysulfone Hemodialyzer 2.2 m2, Low Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS100R</t>
   </si>
   <si>
-    <t>NephroPS100R- Polysulfone Hemodialyzer 1.0 m2, High Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS130R</t>
   </si>
   <si>
-    <t>NephroPS130R- Polysulfone Hemodialyzer 1.3 m2, High Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS140R</t>
   </si>
   <si>
-    <t>NephroPS140R- Polysulfone Hemodialyzer 1.4 m2, High Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS160R</t>
   </si>
   <si>
-    <t>NephroPS160R- Polysulfone Hemodialyzer 1.6 m2, High Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS180R</t>
   </si>
   <si>
-    <t>NephroPS180R- Polysulfone Hemodialyzer 1.8 m2, High Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS200R</t>
   </si>
   <si>
-    <t>NephroPS200R- Polysulfone Hemodialyzer 2.0 m2, High Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>NephroPS220R</t>
   </si>
   <si>
-    <t>NephroPS220R- Polysulfone Hemodialyzer 2.2 m2, High Flux, Sterilized by Gamma</t>
-  </si>
-  <si>
     <t>Product Group</t>
   </si>
   <si>
@@ -143,615 +101,297 @@
     <t>NephroLineU</t>
   </si>
   <si>
-    <t>NephroLineU, Universal Model, without Drain Bag -ETO Sterilized, DEHP Contain</t>
-  </si>
-  <si>
-    <t>NephroLineU, Universal Model, without Drain Bag -ETO Sterilized, DEHP Free</t>
-  </si>
-  <si>
-    <t>NephroLineU, Universal Model, without Drain Bag -Gamma Sterilized, DEHP Free</t>
-  </si>
-  <si>
     <t>NephroLineU+B</t>
   </si>
   <si>
-    <t>NephroLineU+B, Universal Model, with Spike and Drain Bag -ETO Sterilized, DEHP Contain</t>
-  </si>
-  <si>
-    <t>NephroLineU+B, Universal Model, with Spike and Drain Bag -ETO Sterilized, DEHP Free</t>
-  </si>
-  <si>
-    <t>NephroLineU+B, Universal Model, with Spike and Drain Bag -Gamma Sterilized, DEHP Free</t>
-  </si>
-  <si>
     <t xml:space="preserve">NephroLineB </t>
   </si>
   <si>
-    <t>NephroLineB, B-Braun Model, without Drain Bag -ETO Sterilized, DEHP Contain</t>
-  </si>
-  <si>
     <t>NephroLineB+B</t>
   </si>
   <si>
-    <t>NephroLineB+B, B-Braun Model, with Drain Bag -ETO Sterilized, DEHP Contain (B003)</t>
-  </si>
-  <si>
-    <t>NephroLineB+B, B-Braun Model, with Drain Bag -ETO Sterilized, DEHP Contain. (B008)</t>
-  </si>
-  <si>
-    <t>NephroLineB+B, B-Braun Model, with Drain Bag -ETO Sterilized, DEHP Free</t>
-  </si>
-  <si>
-    <t>NephroLineB+B, B-Braun Model, with Drain Bag, -Gamma Sterilized, DEHP Free</t>
-  </si>
-  <si>
     <t xml:space="preserve">NephroLineG </t>
   </si>
   <si>
-    <t>NephroLineG, Gambro Model, Without Drain bag -ETO Sterilized, DEHP Contain</t>
-  </si>
-  <si>
     <t>NephroLineG+B</t>
   </si>
   <si>
-    <t>NephroLineG+B, Gambro Model, with Drain bag -ETO Sterilized, DEHP Contain</t>
-  </si>
-  <si>
-    <t>NephroLineG+B, Gambro Model, with Drain bag -ETO Sterilized, DEHP Free</t>
-  </si>
-  <si>
-    <t>NephroLineG+B, Gambro Model, with Drain bag -Gamma Sterilized, DEHP Free</t>
-  </si>
-  <si>
     <t xml:space="preserve">NephroLineF </t>
   </si>
   <si>
-    <t>NephroLineF, Fresenius Model, without Drain Bag,  -ETO Sterilized, DEHP Contain</t>
-  </si>
-  <si>
     <t>NephroLineF+B</t>
   </si>
   <si>
-    <t>NephroLineF+B, Fresenius Model, with Drain Bag -ETO Sterilized, DEHP Contain</t>
-  </si>
-  <si>
-    <t>NephroLineF+B, Fresenius Model, with Drain Bag -ETO Sterilized, DEHP Free</t>
-  </si>
-  <si>
-    <t>NephroLineF+B, Fresenius Model, with Drain Bag -Gamma Sterilized, DEHP Free</t>
-  </si>
-  <si>
     <t>NephroLineU U001</t>
   </si>
   <si>
-    <t>NephroLine U, Universal model, without Drain Bag, EO sterilized, DEHP Contain (U001)</t>
-  </si>
-  <si>
     <t>NephroLineU U002</t>
   </si>
   <si>
-    <t>NephroLine U, Universal model, without Drain Bag, EO sterilized, DEHP Free (U002)</t>
-  </si>
-  <si>
     <t>NephroLineU U003</t>
   </si>
   <si>
-    <t>NephroLine U, Universal Model, without Drain Bag, Gamma Sterilized, DEHP Contain (U003)</t>
-  </si>
-  <si>
     <t>NephroLineU U004</t>
   </si>
   <si>
-    <t>NephroLine U, Universal Model, without Drain Bag, Gamma Sterilized, DEHP Free (U004)</t>
-  </si>
-  <si>
     <t>NephroLineU+B U005</t>
   </si>
   <si>
-    <t>NephroLine U+B, Universal model, with spike and Drain Bag, EO sterilized, DEHP Contain (U005)</t>
-  </si>
-  <si>
     <t>NephroLineU+B U006</t>
   </si>
   <si>
-    <t>NephroLine U+B, Universal Model, with Spike and Drain Bag, Pump Segment (12.0*8.0*330mm), ETO Sterilized, DEHP Contain (U006)</t>
-  </si>
-  <si>
     <t>NephroLineU+B U008</t>
   </si>
   <si>
-    <t>NephroLine U+B, Universal model, with spike and Drain Bag, EO sterilized, DEHP Free (U008)</t>
-  </si>
-  <si>
     <t>NephroLineU+B U009</t>
   </si>
   <si>
-    <t>NephroLine U+B, Universal Model, with Spike and Drain Bag -Gamma Sterilized, DEHP Contain (U009)</t>
-  </si>
-  <si>
     <t>NephroLineU+B U010</t>
   </si>
   <si>
-    <t>NephroLine U+B, Universal Model, with Spike and Drain Bag -Gamma Sterilized, DEHP Free (U010)</t>
-  </si>
-  <si>
     <t>NephroLineU+B U011</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>NephroLineB B001</t>
   </si>
   <si>
-    <t>NephroLine B, B-Braun Model, without Drain Bag, EO sterilized, DEHP Contain (B001)</t>
-  </si>
-  <si>
     <t>NephroLineB B002</t>
   </si>
   <si>
-    <t>NephroLine B, B-Braun Model, without Drain Bag-Gamma Sterilized, DEHP Contain (B002)</t>
-  </si>
-  <si>
     <t>NephroLineB+B B003</t>
   </si>
   <si>
-    <t>NephroLine B+B, B-Braun Model, with Drain Bag, EO sterilized, DEHP Contain (B003) "Kyrgyzstan"</t>
-  </si>
-  <si>
     <t>NephroLineB+B B004</t>
   </si>
   <si>
-    <t>NephroLine B+B, B-Braun Model, with Drain Bag, EO sterilized, DEHP Free (B004)</t>
-  </si>
-  <si>
     <t>NephroLineB+B B006</t>
   </si>
   <si>
-    <t>NephroLine B+B, B-Braun Model, with Drain Bag - Gamma Sterilized, DEHP Contain (B006)</t>
-  </si>
-  <si>
     <t>NephroLineB+B B007</t>
   </si>
   <si>
-    <t>NephroLine B+B, B-Braun Model, with Drain Bag -Gamma Sterilized, DEHP Free (B007)</t>
-  </si>
-  <si>
     <t>NephroLineB+B B008</t>
   </si>
   <si>
-    <t>NephroLine B+B, B-Braun Model, with Drain Bag, EO sterilized, DEHP Contain (B008) "Lebanon"</t>
-  </si>
-  <si>
     <t>NephroLineB+B B009</t>
   </si>
   <si>
-    <t>NephroLine B+B, B-Braun Model, with Drain Bag -Gamma Sterilized, DEHP-Free (B009) "Lebanon"</t>
-  </si>
-  <si>
     <t>NephroLineB+B B010</t>
   </si>
   <si>
-    <t>NephroLine B+B, B-Braun Model, with Drain Bag -Gamma Sterilized, DEHP-Free (B010) "Lebanon"</t>
-  </si>
-  <si>
     <t>NephroLineG G001</t>
   </si>
   <si>
-    <t>NephroLine G, Gambro Model, without Drain Bag, EO sterilized, DEHP Contain (G001)</t>
-  </si>
-  <si>
     <t>NephroLineG G002</t>
   </si>
   <si>
-    <t>NephroLine G, Gambro Model, without Drain bag-Gamma Sterilized, DEHP Contain (G002)</t>
-  </si>
-  <si>
     <t>NephroLineG+B G003</t>
   </si>
   <si>
-    <t>NephroLine G+B, Gambro Model, with Drain Bag, EO sterilized, DEHP Contain (G003)</t>
-  </si>
-  <si>
     <t>NephroLineG+B G004</t>
   </si>
   <si>
-    <t>NephroLine G+B, Gambro Model, with Drain Bag, EO sterilized, DEHP Free (G004)</t>
-  </si>
-  <si>
     <t>NephroLineG+B G005</t>
   </si>
   <si>
-    <t>NephroLine G+B, Gambro Model, with Drain bag - Gamma Sterilized, DEHP Contain (G005)</t>
-  </si>
-  <si>
     <t>NephroLineG+B G006</t>
   </si>
   <si>
-    <t>NephroLine G+B, Gambro Model, with Drain bag, Gamma Sterilized, DEHP Free (G006)</t>
-  </si>
-  <si>
     <t>NephroLineG+B G007</t>
   </si>
   <si>
-    <t>NephroLine G+B, Gambro Model, with Drain bag, Gamma Sterilized, DEHP Free (G007) "Lebanon"</t>
-  </si>
-  <si>
     <t>NephroLineF F001</t>
   </si>
   <si>
-    <t>NephroLine F, Fresenius Model, without Drain Bag, EO sterilized, DEHP Contain (F001)</t>
-  </si>
-  <si>
     <t>NephroLineF F002</t>
   </si>
   <si>
-    <t>NephroLine F, Fresenius Model, without Drain Bag, -Gamma Sterilized, DEHP Contain (F002)</t>
-  </si>
-  <si>
     <t>NephroLineF+B F003</t>
   </si>
   <si>
-    <t>NephroLine F+B, Fresenius Model, with Drain Bag, EO sterilized, DEHP Contain (F003)</t>
-  </si>
-  <si>
     <t>NephroLineF+B F012</t>
   </si>
   <si>
-    <t>NephroLine F+B, Fresenius Model, with Drain Bag, EO sterilized, DEHP Contain (F012) "Different tube dimension"</t>
-  </si>
-  <si>
     <t>NephroLineF+B F008</t>
   </si>
   <si>
-    <t>NephroLine F+B, Fresenius Model, with Drain Bag, Pump Segment (12.0*8.0*330 mm), ETO Sterilized, DEHP Contain (F008)</t>
-  </si>
-  <si>
     <t>NephroLineF+B F009</t>
   </si>
   <si>
-    <t>NephroLine F+B, Fresenius Model, with Drain Bag, EO sterilized, DEHP Free (F009)</t>
-  </si>
-  <si>
     <t>NephroLineF+B F010</t>
   </si>
   <si>
-    <t>NephroLine F+B, Fresenius Model, with Drain Bag - Gamma Sterilized, DEHP Contain (F010)</t>
-  </si>
-  <si>
     <t>NephroLineF+B F011</t>
   </si>
   <si>
-    <t>NephroLine F+B, Fresenius Model, with Drain Bag - Gamma Sterilized, DEHP Free (F011)</t>
-  </si>
-  <si>
     <t>NephroLineN N001</t>
   </si>
   <si>
-    <t>NephroLine N, Nippro Model, with spike and without Drain Bag, EO sterilized, DEHP Free (N001)</t>
-  </si>
-  <si>
     <t>NephroLineN N002</t>
   </si>
   <si>
-    <t>NephroLine N, Nippro Model, with Spike and without Drain Bag, Gamma Sterilized, DEHP Free (N002)</t>
-  </si>
-  <si>
     <t>NephroLineK+B K001</t>
   </si>
   <si>
-    <t>NephroLine K+B, Nikkiso Model, with Drain Bag, EO sterilized, DEHP Free (K001)</t>
-  </si>
-  <si>
     <t>NephroLineK+B K002</t>
   </si>
   <si>
-    <t>NephroLine K+B, Nikkiso Model, with Drain Bag, Gamma Sterilized, DEHP Free (K002)</t>
-  </si>
-  <si>
     <t>NEEDLE</t>
   </si>
   <si>
     <t>NephroNeedle15ASE</t>
   </si>
   <si>
-    <t>NephroNeedle15ASE, Fistula Needle, Arterial Line, 15G (1.8 * 25 mm) 150 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle15VSE</t>
   </si>
   <si>
-    <t>NephroNeedle15VSE, Fistula Needle, Venous line, 15G (1.8 * 25 mm) 150 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle15AVSE</t>
   </si>
   <si>
-    <t>NephroNeedle15AVSE, Fistula Needle Set, Arterial+ Venous Line, 15G (1.8 * 25 mm) 150 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle15ASR</t>
   </si>
   <si>
-    <t>NephroNeedle15ASR, Fistula Needle, Arterial Line, 15G (1.8 * 25 mm) 150 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle15VSR</t>
   </si>
   <si>
-    <t>NephroNeedle15VSR, Fistula Needle, Venous line, 15G (1.8 * 25 mm) 150 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle15AVSR</t>
   </si>
   <si>
-    <t>NephroNeedle15AVSR, Fistula Needle Set, Arterial+ Venous Line, 15G (1.8 * 25 mm) 150 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle15ALE</t>
   </si>
   <si>
-    <t>NephroNeedle15ALE, Fistula Needle, Arterial Line, 15G (1.8 * 25 mm) 300 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle15VLE</t>
   </si>
   <si>
-    <t>NephroNeedle15VLE, Fistula Needle, Venous line, 15G (1.8 * 25 mm) 300 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle15AVLE</t>
   </si>
   <si>
-    <t>NephroNeedle15AVLE, Fistula Needle Set, Arterial+ Venous Line, 15G (1.8 * 25 mm) 300 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle15ALR</t>
   </si>
   <si>
-    <t>NephroNeedle15ALR, Fistula Needle, Arterial Line, 15G (1.8 * 25 mm) 300 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle15VLR</t>
   </si>
   <si>
-    <t>NephroNeedle15VLR, Fistula Needle, Venous line, 15G (1.8 * 25 mm) 300 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle15AVLR</t>
   </si>
   <si>
-    <t>NephroNeedle15AVLR, Fistula Needle, Arterial+ Venous Line, 15G (1.8 * 25 mm) 300 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle16ASE</t>
   </si>
   <si>
-    <t>NephroNeedle16ASE, Fistula Needle, Arterial Line, 16G (1.6 * 25 mm) 150 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle16VSE</t>
   </si>
   <si>
-    <t>NephroNeedle16VSE, Fistula Needle, Venous line, 16G (1.6 * 25 mm) 150 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle16AVSE</t>
   </si>
   <si>
-    <t>NephroNeedle16AVSE, Fistula Needle Set, Arterial+ Venous Line, 16G (1.6 * 25 mm) 150 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle16ASR</t>
   </si>
   <si>
-    <t>NephroNeedle16ASR, Fistula Needle, Arterial Line, 16G (1.6 * 25 mm) 150 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle16VSR</t>
   </si>
   <si>
-    <t>NephroNeedle16VSR, Fistula Needle, Venous line, 16G (1.6 * 25 mm) 150 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle16AVSR</t>
   </si>
   <si>
-    <t>NephroNeedle16AVSR, Fistula Needle Set, Arterial+ Venous Line, 16G (1.6 * 25 mm) 150 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle16ALE</t>
   </si>
   <si>
-    <t>NephroNeedle16ALE, Fistula Needle, Arterial Line, 16G (1.6 * 25 mm) 300 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle16VLE</t>
   </si>
   <si>
-    <t>NephroNeedle16VLE, Fistula Needle, Venous line, 16G (1.6 * 25 mm) 300 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle16AVLE</t>
   </si>
   <si>
-    <t>NephroNeedle16AVLE, Fistula Needle Set, Arterial+ Venous Line, 16G (1.6 * 25 mm) 300 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle16ALR</t>
   </si>
   <si>
-    <t>NephroNeedle16ALR, Fistula Needle, Arterial Line, 16G (1.6 * 25 mm) 300 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle16VLR</t>
   </si>
   <si>
-    <t>NephroNeedle16VLR, Fistula Needle, Venous line, 16G (1.6 * 25 mm) 300 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle16AVLR</t>
   </si>
   <si>
-    <t>NephroNeedle16AVLR, Fistula Needle, Arterial+ Venous Line, 16G (1.6 * 25 mm) 300 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle17ASE</t>
   </si>
   <si>
-    <t>NephroNeedle17ASE, Fistula Needle, Arterial Line, 17G (1.4 * 25 mm) 150 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle17VSE</t>
   </si>
   <si>
-    <t>NephroNeedle17VSE, Fistula Needle, Venous line, 17G (1.4 * 25 mm) 150 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle17AVSE</t>
   </si>
   <si>
-    <t>NephroNeedle17AVSE, Fistula Needle, Arterial+ Venous Line, 17G (1.4 * 25 mm) 150 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle17ASR</t>
   </si>
   <si>
-    <t>NephroNeedle17ASR, Fistula Needle, Arterial Line, 17G (1.4 * 25 mm) 150 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle17VSR</t>
   </si>
   <si>
-    <t>NephroNeedle17VSR, Fistula Needle, Venous line, 17G (1.4 * 25 mm) 150 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle17AVSR</t>
   </si>
   <si>
-    <t>NephroNeedle17AVSR, Fistula Needle, Arterial+ Venous Line, 17G (1.4 * 25 mm) 150 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle17ALE</t>
   </si>
   <si>
-    <t>NephroNeedle17ALE, Fistula Needle, Arterial Line, 17G (1.4 * 25 mm) 300 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle17VLE</t>
   </si>
   <si>
-    <t>NephroNeedle17VLE, Fistula Needle, Venous line, 17G (1.4 * 25 mm) 300 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle17AVLE</t>
   </si>
   <si>
-    <t>NephroNeedle17AVLE, Fistula Needle, Arterial+ Venous Line, 17G (1.4 * 25 mm) 300 mm, Sterilized with EO</t>
-  </si>
-  <si>
     <t>NephroNeedle17ALR</t>
   </si>
   <si>
-    <t>NephroNeedle17ALR, Fistula Needle, Arterial Line, 17G (1.4 * 25 mm) 300 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle17VLR</t>
   </si>
   <si>
-    <t>NephroNeedle17VLR, Fistula Needle, Venous line, 17G (1.4 * 25 mm) 300 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>NephroNeedle17AVLR</t>
   </si>
   <si>
-    <t>NephroNeedle17AVLR, Fistula Needle, Arterial+ Venous Line, 17G (1.4 * 25 mm) 300 mm, Sterilized with Gamma</t>
-  </si>
-  <si>
     <t>POWDER</t>
   </si>
   <si>
     <t>NephroBag650</t>
   </si>
   <si>
-    <t>NephroBag650, Sodium Bicarbonate Bag 650 gr</t>
-  </si>
-  <si>
     <t>NephroBag750</t>
   </si>
   <si>
-    <t>NephroBag750, Sodium Bicarbonate Bag 750 gr</t>
-  </si>
-  <si>
     <t>NephroCart650</t>
   </si>
   <si>
-    <t>NephroCart650, Sodium Bicarbonate Cartridge 650 gr</t>
-  </si>
-  <si>
     <t>NephroCart750</t>
   </si>
   <si>
-    <t>NephroCart750, Sodium Bicarbonate Cartridge 750 gr</t>
-  </si>
-  <si>
     <t>MACHINERY</t>
   </si>
   <si>
     <t>NephroCRO - NCS1</t>
   </si>
   <si>
-    <t>NephroCRO - NCS1, Single pass RO machine for hemodialysis application. This model has a membrane</t>
-  </si>
-  <si>
     <t>NephroCRO - NCS2</t>
   </si>
   <si>
-    <t>NephroCRO - NCS2, Single pass RO machine for hemodialysis application. This model has two membranes</t>
-  </si>
-  <si>
     <t>NephroCRO - NCS3</t>
   </si>
   <si>
-    <t>NephroCRO - NCS3, Single pass RO machine for hemodialysis application. This model has three membranes</t>
-  </si>
-  <si>
     <t>NephroCRO - NCS4</t>
   </si>
   <si>
-    <t>NephroCRO - NCS4, Single pass RO machine for hemodialysis application. This model has four membranes</t>
-  </si>
-  <si>
     <t>NephroCRO - NDS1</t>
   </si>
   <si>
-    <t>NephroCRO - NDS1, Double pass RO machine for hemodialysis application. This model has two membranes in the first pass and one membrane in second pass</t>
-  </si>
-  <si>
     <t>NephroCRO - NDS2</t>
   </si>
   <si>
-    <t>NephroCRO - NDS2, Double pass RO machine for hemodialysis application. This model has three membranes in the first pass and two membranes in second pass</t>
-  </si>
-  <si>
     <t>NephroCRO - NDS3</t>
   </si>
   <si>
-    <t>NephroCRO - NDS3, Double pass RO machine for hemodialysis application. This model has four membranes in the first pass and three membranes in second pass</t>
-  </si>
-  <si>
     <t>NephroCRO - NDS4</t>
   </si>
   <si>
-    <t>NephroCRO - NDS4, Double pass RO machine for hemodialysis application. This model has five membranes in the first pass and four membranes in second pass</t>
-  </si>
-  <si>
     <t>NephroPRO - NPS1</t>
   </si>
   <si>
-    <t>NephroPRO - NPS1, Single pass portable RO machine for hemodialysis application. This model has just one membrane</t>
-  </si>
-  <si>
     <t>NephroHDM</t>
   </si>
   <si>
@@ -761,23 +401,383 @@
     <t>NephroChair-NDC1</t>
   </si>
   <si>
-    <t>NephroChair-NDC1- without weighing system</t>
-  </si>
-  <si>
     <t>NephroChair-NDC2</t>
   </si>
   <si>
-    <t>NephroChair-NDC2- with weighing system</t>
-  </si>
-  <si>
     <t>DIALYZER</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 1.0 m2, Low Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 1.3 m2, Low Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 1.4 m2, Low Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 1.6 m2, Low Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 1.8 m2, Low Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 2.0 m2, Low Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 2.2 m2, Low Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 1.0 m2, High Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 1.3 m2, High Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 1.4 m2, High Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 1.6 m2, High Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 1.8 m2, High Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 2.0 m2, High Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Polysulfone Hemodialyzer 2.2 m2, High Flux, Sterilized by Gamma</t>
+  </si>
+  <si>
+    <t>Universal Model, without Drain Bag -ETO Sterilized, DEHP Contain</t>
+  </si>
+  <si>
+    <t>Universal Model, without Drain Bag -ETO Sterilized, DEHP Free</t>
+  </si>
+  <si>
+    <t>Universal Model, without Drain Bag -Gamma Sterilized, DEHP Free</t>
+  </si>
+  <si>
+    <t>Universal Model, with Spike and Drain Bag -ETO Sterilized, DEHP Contain</t>
+  </si>
+  <si>
+    <t>Universal Model, with Spike and Drain Bag -ETO Sterilized, DEHP Free</t>
+  </si>
+  <si>
+    <t>Universal Model, with Spike and Drain Bag -Gamma Sterilized, DEHP Free</t>
+  </si>
+  <si>
+    <t>B-Braun Model, without Drain Bag -ETO Sterilized, DEHP Contain</t>
+  </si>
+  <si>
+    <t>B-Braun Model, with Drain Bag -ETO Sterilized, DEHP Contain (B003)</t>
+  </si>
+  <si>
+    <t>B-Braun Model, with Drain Bag -ETO Sterilized, DEHP Contain. (B008)</t>
+  </si>
+  <si>
+    <t>B-Braun Model, with Drain Bag -ETO Sterilized, DEHP Free</t>
+  </si>
+  <si>
+    <t>B-Braun Model, with Drain Bag, -Gamma Sterilized, DEHP Free</t>
+  </si>
+  <si>
+    <t>Gambro Model, Without Drain bag -ETO Sterilized, DEHP Contain</t>
+  </si>
+  <si>
+    <t>Gambro Model, with Drain bag -ETO Sterilized, DEHP Contain</t>
+  </si>
+  <si>
+    <t>Gambro Model, with Drain bag -ETO Sterilized, DEHP Free</t>
+  </si>
+  <si>
+    <t>Gambro Model, with Drain bag -Gamma Sterilized, DEHP Free</t>
+  </si>
+  <si>
+    <t>Fresenius Model, without Drain Bag,  -ETO Sterilized, DEHP Contain</t>
+  </si>
+  <si>
+    <t>Fresenius Model, with Drain Bag -ETO Sterilized, DEHP Contain</t>
+  </si>
+  <si>
+    <t>Fresenius Model, with Drain Bag -ETO Sterilized, DEHP Free</t>
+  </si>
+  <si>
+    <t>Fresenius Model, with Drain Bag -Gamma Sterilized, DEHP Free</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial Line, 15G (1.8 * 25 mm) 150 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Venous line, 15G (1.8 * 25 mm) 150 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle Set, Arterial+ Venous Line, 15G (1.8 * 25 mm) 150 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial Line, 15G (1.8 * 25 mm) 150 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Venous line, 15G (1.8 * 25 mm) 150 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle Set, Arterial+ Venous Line, 15G (1.8 * 25 mm) 150 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial Line, 15G (1.8 * 25 mm) 300 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Venous line, 15G (1.8 * 25 mm) 300 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle Set, Arterial+ Venous Line, 15G (1.8 * 25 mm) 300 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial Line, 15G (1.8 * 25 mm) 300 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Venous line, 15G (1.8 * 25 mm) 300 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial+ Venous Line, 15G (1.8 * 25 mm) 300 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial Line, 16G (1.6 * 25 mm) 150 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Venous line, 16G (1.6 * 25 mm) 150 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle Set, Arterial+ Venous Line, 16G (1.6 * 25 mm) 150 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial Line, 16G (1.6 * 25 mm) 150 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Venous line, 16G (1.6 * 25 mm) 150 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle Set, Arterial+ Venous Line, 16G (1.6 * 25 mm) 150 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial Line, 16G (1.6 * 25 mm) 300 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Venous line, 16G (1.6 * 25 mm) 300 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle Set, Arterial+ Venous Line, 16G (1.6 * 25 mm) 300 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial Line, 16G (1.6 * 25 mm) 300 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Venous line, 16G (1.6 * 25 mm) 300 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial+ Venous Line, 16G (1.6 * 25 mm) 300 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial Line, 17G (1.4 * 25 mm) 150 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Venous line, 17G (1.4 * 25 mm) 150 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial+ Venous Line, 17G (1.4 * 25 mm) 150 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial Line, 17G (1.4 * 25 mm) 150 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Venous line, 17G (1.4 * 25 mm) 150 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial+ Venous Line, 17G (1.4 * 25 mm) 150 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial Line, 17G (1.4 * 25 mm) 300 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Venous line, 17G (1.4 * 25 mm) 300 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial+ Venous Line, 17G (1.4 * 25 mm) 300 mm, Sterilized with EO</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial Line, 17G (1.4 * 25 mm) 300 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Venous line, 17G (1.4 * 25 mm) 300 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Fistula Needle, Arterial+ Venous Line, 17G (1.4 * 25 mm) 300 mm, Sterilized with Gamma</t>
+  </si>
+  <si>
+    <t>Sodium Bicarbonate Bag 650 gr</t>
+  </si>
+  <si>
+    <t>Sodium Bicarbonate Bag 750 gr</t>
+  </si>
+  <si>
+    <t>Sodium Bicarbonate Cartridge 650 gr</t>
+  </si>
+  <si>
+    <t>Sodium Bicarbonate Cartridge 750 gr</t>
+  </si>
+  <si>
+    <t>NCS1, Single pass RO machine for hemodialysis application. This model has a membrane</t>
+  </si>
+  <si>
+    <t>NCS2, Single pass RO machine for hemodialysis application. This model has two membranes</t>
+  </si>
+  <si>
+    <t>NCS3, Single pass RO machine for hemodialysis application. This model has three membranes</t>
+  </si>
+  <si>
+    <t>NCS4, Single pass RO machine for hemodialysis application. This model has four membranes</t>
+  </si>
+  <si>
+    <t>NDS1, Double pass RO machine for hemodialysis application. This model has two membranes in the first pass and one membrane in second pass</t>
+  </si>
+  <si>
+    <t>NDS2, Double pass RO machine for hemodialysis application. This model has three membranes in the first pass and two membranes in second pass</t>
+  </si>
+  <si>
+    <t>NDS3, Double pass RO machine for hemodialysis application. This model has four membranes in the first pass and three membranes in second pass</t>
+  </si>
+  <si>
+    <t>NDS4, Double pass RO machine for hemodialysis application. This model has five membranes in the first pass and four membranes in second pass</t>
+  </si>
+  <si>
+    <t>NPS1, Single pass portable RO machine for hemodialysis application. This model has just one membrane</t>
+  </si>
+  <si>
+    <t>DC1- without weighing system</t>
+  </si>
+  <si>
+    <t>DC2- with weighing system</t>
+  </si>
+  <si>
+    <t>Universal model, without Drain Bag, EO sterilized, DEHP Contain (U001)</t>
+  </si>
+  <si>
+    <t>Universal model, without Drain Bag, EO sterilized, DEHP Free (U002)</t>
+  </si>
+  <si>
+    <t>Universal Model, without Drain Bag, Gamma Sterilized, DEHP Contain (U003)</t>
+  </si>
+  <si>
+    <t>Universal Model, without Drain Bag, Gamma Sterilized, DEHP Free (U004)</t>
+  </si>
+  <si>
+    <t>Universal model, with spike and Drain Bag, EO sterilized, DEHP Contain (U005)</t>
+  </si>
+  <si>
+    <t>Universal Model, with Spike and Drain Bag, Pump Segment (12.0*8.0*330mm), ETO Sterilized, DEHP Contain (U006)</t>
+  </si>
+  <si>
+    <t>Universal model, with spike and Drain Bag, EO sterilized, DEHP Free (U008)</t>
+  </si>
+  <si>
+    <t>Universal Model, with Spike and Drain Bag -Gamma Sterilized, DEHP Contain (U009)</t>
+  </si>
+  <si>
+    <t>Universal Model, with Spike and Drain Bag -Gamma Sterilized, DEHP Free (U010)</t>
+  </si>
+  <si>
+    <t>Universal Model, with Spike and Drain Bag -Gamma Sterilized, DEHP Free (U011)</t>
+  </si>
+  <si>
+    <t>B-Braun Model, without Drain Bag, EO sterilized, DEHP Contain (B001)</t>
+  </si>
+  <si>
+    <t>B-Braun Model, without Drain Bag-Gamma Sterilized, DEHP Contain (B002)</t>
+  </si>
+  <si>
+    <t>B-Braun Model, with Drain Bag, EO sterilized, DEHP Contain (B003)</t>
+  </si>
+  <si>
+    <t>B-Braun Model, with Drain Bag, EO sterilized, DEHP Free (B004)</t>
+  </si>
+  <si>
+    <t>B-Braun Model, with Drain Bag - Gamma Sterilized, DEHP Contain (B006)</t>
+  </si>
+  <si>
+    <t>B-Braun Model, with Drain Bag -Gamma Sterilized, DEHP Free (B007)</t>
+  </si>
+  <si>
+    <t>B-Braun Model, with Drain Bag, EO sterilized, DEHP Contain (B008)</t>
+  </si>
+  <si>
+    <t>B-Braun Model, with Drain Bag -Gamma Sterilized, DEHP-Free (B009)</t>
+  </si>
+  <si>
+    <t>B-Braun Model, with Drain Bag -Gamma Sterilized, DEHP-Free (B010)</t>
+  </si>
+  <si>
+    <t>Gambro Model, without Drain Bag, EO sterilized, DEHP Contain (G001)</t>
+  </si>
+  <si>
+    <t>Gambro Model, without Drain bag-Gamma Sterilized, DEHP Contain (G002)</t>
+  </si>
+  <si>
+    <t>Gambro Model, with Drain Bag, EO sterilized, DEHP Contain (G003)</t>
+  </si>
+  <si>
+    <t>Gambro Model, with Drain Bag, EO sterilized, DEHP Free (G004)</t>
+  </si>
+  <si>
+    <t>Gambro Model, with Drain bag - Gamma Sterilized, DEHP Contain (G005)</t>
+  </si>
+  <si>
+    <t>Gambro Model, with Drain bag, Gamma Sterilized, DEHP Free (G006)</t>
+  </si>
+  <si>
+    <t>Gambro Model, with Drain bag, Gamma Sterilized, DEHP Free (G007)</t>
+  </si>
+  <si>
+    <t>Fresenius Model, without Drain Bag, EO sterilized, DEHP Contain (F001)</t>
+  </si>
+  <si>
+    <t>Fresenius Model, without Drain Bag, -Gamma Sterilized, DEHP Contain (F002)</t>
+  </si>
+  <si>
+    <t>Fresenius Model, with Drain Bag, EO sterilized, DEHP Contain (F003)</t>
+  </si>
+  <si>
+    <t>Fresenius Model, with Drain Bag, EO sterilized, DEHP Contain (F012)</t>
+  </si>
+  <si>
+    <t>Fresenius Model, with Drain Bag, Pump Segment (12.0*8.0*330 mm), ETO Sterilized, DEHP Contain (F008)</t>
+  </si>
+  <si>
+    <t>Fresenius Model, with Drain Bag, EO sterilized, DEHP Free (F009)</t>
+  </si>
+  <si>
+    <t>Fresenius Model, with Drain Bag - Gamma Sterilized, DEHP Contain (F010)</t>
+  </si>
+  <si>
+    <t>Fresenius Model, with Drain Bag - Gamma Sterilized, DEHP Free (F011)</t>
+  </si>
+  <si>
+    <t>Nippro Model, with spike and without Drain Bag, EO sterilized, DEHP Free (N001)</t>
+  </si>
+  <si>
+    <t>Nippro Model, with Spike and without Drain Bag, Gamma Sterilized, DEHP Free (N002)</t>
+  </si>
+  <si>
+    <t>Nikkiso Model, with Drain Bag, EO sterilized, DEHP Free (K001)</t>
+  </si>
+  <si>
+    <t>Nikkiso Model, with Drain Bag, Gamma Sterilized, DEHP Free (K002)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -803,6 +803,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -853,7 +859,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -873,6 +879,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1210,14 +1219,18 @@
   <dimension ref="A1:D176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="4" max="4" width="85.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1229,9 +1242,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -1240,701 +1253,701 @@
         <v>4210217</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="136" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>5</v>
       </c>
       <c r="C3" s="6">
         <v>4210222</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4">
         <v>4210247</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6">
         <v>4210227</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4">
         <v>4210232</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C7" s="6">
         <v>4210237</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4">
         <v>4210242</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C9" s="6">
         <v>4210257</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C10" s="4">
         <v>4210262</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C11" s="6">
         <v>4210287</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C12" s="4">
         <v>4210267</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C13" s="6">
         <v>4210272</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C14" s="4">
         <v>4210277</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>243</v>
+        <v>121</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C15" s="6">
         <v>4210282</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C16" s="4">
         <v>4212205</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C17" s="6">
         <v>4212220</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C18" s="4">
         <v>4212223</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C19" s="6">
         <v>4212305</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C20" s="4">
         <v>4212320</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C21" s="6">
         <v>4212323</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C22" s="4">
         <v>4212408</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C23" s="6">
         <v>4212405</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C24" s="4">
         <v>4212405</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C25" s="6">
         <v>4212420</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C26" s="4">
         <v>4212423</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C27" s="6">
         <v>4212508</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C28" s="4">
         <v>4212505</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C29" s="6">
         <v>4212520</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C30" s="4">
         <v>4212523</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="C31" s="6">
         <v>4212708</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C32" s="4">
         <v>4212705</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C33" s="6">
         <v>4212720</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C34" s="4">
         <v>4212723</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>137</v>
+        <v>66</v>
       </c>
       <c r="C35" s="6">
         <v>4218304</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="C36" s="4">
         <v>4218307</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>141</v>
+        <v>68</v>
       </c>
       <c r="C37" s="6">
         <v>4218310</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>143</v>
+        <v>69</v>
       </c>
       <c r="C38" s="4">
         <v>4218314</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="C39" s="6">
         <v>4218317</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>147</v>
+        <v>71</v>
       </c>
       <c r="C40" s="4">
         <v>4218320</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>149</v>
+        <v>72</v>
       </c>
       <c r="C41" s="6">
         <v>4218324</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>151</v>
+        <v>73</v>
       </c>
       <c r="C42" s="4">
         <v>4218327</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>153</v>
+        <v>74</v>
       </c>
       <c r="C43" s="6">
         <v>4218330</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>155</v>
+        <v>75</v>
       </c>
       <c r="C44" s="4">
         <v>4218334</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>157</v>
+        <v>76</v>
       </c>
       <c r="C45" s="6">
         <v>4218337</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>159</v>
+        <v>77</v>
       </c>
       <c r="C46" s="4">
         <v>4218340</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>161</v>
+        <v>78</v>
       </c>
       <c r="C47" s="6">
         <v>4218404</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>163</v>
+        <v>79</v>
       </c>
       <c r="C48" s="4">
         <v>4218407</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>165</v>
+        <v>80</v>
       </c>
       <c r="C49" s="6">
         <v>4218410</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>167</v>
+        <v>81</v>
       </c>
       <c r="C50" s="4">
         <v>4218414</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>169</v>
+        <v>82</v>
       </c>
       <c r="C51" s="6">
         <v>4218417</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>171</v>
+        <v>83</v>
       </c>
       <c r="C52" s="4">
         <v>4218420</v>
@@ -1943,1012 +1956,1012 @@
         <v>172</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>173</v>
+        <v>84</v>
       </c>
       <c r="C53" s="6">
         <v>4218424</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>175</v>
+        <v>85</v>
       </c>
       <c r="C54" s="4">
         <v>4218427</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>177</v>
+        <v>86</v>
       </c>
       <c r="C55" s="6">
         <v>4218430</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>179</v>
+        <v>87</v>
       </c>
       <c r="C56" s="4">
         <v>4218434</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>181</v>
+        <v>88</v>
       </c>
       <c r="C57" s="6">
         <v>4218437</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>183</v>
+        <v>89</v>
       </c>
       <c r="C58" s="4">
         <v>4218440</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>185</v>
+        <v>90</v>
       </c>
       <c r="C59" s="6">
         <v>4218504</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>187</v>
+        <v>91</v>
       </c>
       <c r="C60" s="4">
         <v>4218507</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>189</v>
+        <v>92</v>
       </c>
       <c r="C61" s="6">
         <v>4218510</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>191</v>
+        <v>93</v>
       </c>
       <c r="C62" s="4">
         <v>4218514</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>193</v>
+        <v>94</v>
       </c>
       <c r="C63" s="6">
         <v>4218517</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>195</v>
+        <v>95</v>
       </c>
       <c r="C64" s="4">
         <v>4218520</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>197</v>
+        <v>96</v>
       </c>
       <c r="C65" s="6">
         <v>4218524</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>199</v>
+        <v>97</v>
       </c>
       <c r="C66" s="4">
         <v>4218527</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>201</v>
+        <v>98</v>
       </c>
       <c r="C67" s="6">
         <v>4218530</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>203</v>
+        <v>99</v>
       </c>
       <c r="C68" s="4">
         <v>4218534</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>205</v>
+        <v>100</v>
       </c>
       <c r="C69" s="6">
         <v>4218537</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>207</v>
+        <v>101</v>
       </c>
       <c r="C70" s="4">
         <v>4218540</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>209</v>
+        <v>102</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>210</v>
+        <v>103</v>
       </c>
       <c r="C71" s="4">
         <v>4315220</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>209</v>
+        <v>102</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>212</v>
+        <v>104</v>
       </c>
       <c r="C72" s="6">
         <v>4315230</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>209</v>
+        <v>102</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>214</v>
+        <v>105</v>
       </c>
       <c r="C73" s="6">
         <v>4315320</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>209</v>
+        <v>102</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>216</v>
+        <v>106</v>
       </c>
       <c r="C74" s="4">
         <v>4315330</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>219</v>
+        <v>108</v>
       </c>
       <c r="C75" s="6">
         <v>4620110</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>221</v>
+        <v>109</v>
       </c>
       <c r="C76" s="4">
         <v>4620115</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>223</v>
+        <v>110</v>
       </c>
       <c r="C77" s="6">
         <v>4620120</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>225</v>
+        <v>111</v>
       </c>
       <c r="C78" s="4">
         <v>4620125</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="306" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>227</v>
+        <v>112</v>
       </c>
       <c r="C79" s="6">
         <v>4620155</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="306" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>229</v>
+        <v>113</v>
       </c>
       <c r="C80" s="4">
         <v>4620160</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="306" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>231</v>
+        <v>114</v>
       </c>
       <c r="C81" s="6">
         <v>4620165</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="306" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>233</v>
+        <v>115</v>
       </c>
       <c r="C82" s="4">
         <v>4620170</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>235</v>
+        <v>116</v>
       </c>
       <c r="C83" s="6">
         <v>4620310</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>237</v>
+        <v>117</v>
       </c>
       <c r="C84" s="4">
         <v>10101010101</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>239</v>
+        <v>119</v>
       </c>
       <c r="C85" s="6">
         <v>4640110</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>218</v>
+        <v>107</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>241</v>
+        <v>120</v>
       </c>
       <c r="C86" s="4">
         <v>4640111</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="C87" s="6">
         <v>4212205</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C88" s="4">
         <v>4212220</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="C89" s="10">
         <v>4212225</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C90" s="10">
         <v>4212230</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="C91" s="6">
         <v>4212305</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="255" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="C92" s="4">
         <v>4212310</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="C93" s="6">
         <v>4212320</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="C94" s="10">
         <v>4212325</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="C95" s="10">
         <v>4212330</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>77</v>
+        <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="C96" s="10">
         <v>4212330</v>
       </c>
-      <c r="D96" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="D96" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="C97" s="6">
         <v>4212408</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="C98" s="10">
         <v>4212415</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="C99" s="6">
         <v>4212405</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C100" s="4">
         <v>4212420</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="C101" s="10">
         <v>4212425</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="C102" s="10">
         <v>4212430</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="C103" s="6">
         <v>4212405</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="C104" s="10">
         <v>4212430</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="C105" s="10">
         <v>4212430</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="C106" s="4">
         <v>4212508</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="C107" s="10">
         <v>4212515</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="C108" s="4">
         <v>4212505</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="C109" s="6">
         <v>4212520</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="C110" s="10">
         <v>4212525</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="C111" s="10">
         <v>4212530</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="C112" s="10">
         <v>4212530</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="C113" s="6">
         <v>4212708</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
       <c r="C114" s="10">
         <v>4212715</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="C115" s="6">
         <v>4212705</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>118</v>
+        <v>56</v>
       </c>
       <c r="C116" s="4">
         <v>4212705</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="C117" s="10">
         <v>4212710</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="C118" s="4">
         <v>4212720</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>124</v>
+        <v>59</v>
       </c>
       <c r="C119" s="10">
         <v>4212725</v>
       </c>
       <c r="D119" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>126</v>
+        <v>60</v>
       </c>
       <c r="C120" s="10">
         <v>4212730</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="C121" s="6">
         <v>4213320</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
       <c r="C122" s="4">
         <v>4213330</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="C123" s="6">
         <v>4213420</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="8" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>134</v>
+        <v>64</v>
       </c>
       <c r="C124" s="8">
         <v>4213430</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>135</v>
+        <v>243</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3264,7 +3277,7 @@
       <c r="D176" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{17F5C3D3-4489-534F-B22E-FFEEBED3B745}"/>
+  <autoFilter ref="A1:D124" xr:uid="{17F5C3D3-4489-534F-B22E-FFEEBED3B745}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>